<commit_message>
Last changes for v1.0.2
Last changes for v1.0.2
</commit_message>
<xml_diff>
--- a/seronetTemplates/template/subjectHuman.xlsx
+++ b/seronetTemplates/template/subjectHuman.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liualg/Documents/GitHub/SeroNet/seronetTemplates/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC76195-6745-0349-9527-7C4724B742DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8261617-AE45-3049-8660-24122B363665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="500" windowWidth="34940" windowHeight="15740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="900" yWindow="500" windowWidth="34940" windowHeight="15740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="subjectHumans.txt" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,19 @@
     <definedName name="lookuprace1082">lookup!$A$745:$A$753</definedName>
     <definedName name="lookupsubject_location1080">lookup!$A$480:$A$739</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -307,10 +319,9 @@
         <r>
           <rPr>
             <sz val="11"/>
-            <color indexed="8"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>The NCBI Disease Ontology ID associated with the disease. If the Disease Reported is not a preferred value, then the Disease Ontology ID must be provided. If the disease is a preferred value, then the Disease Ontology ID will be the DOID associated with the preferred value.  The template column is associated with the following database table column immune_exposure.disease_ontology_id and has data type varchar(100)</t>
         </r>
@@ -3076,10 +3087,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V200"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7926,12 +7938,14 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:A753"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>